<commit_message>
feat(uploadEmployeesMinexus): excel read employees
</commit_message>
<xml_diff>
--- a/Analisis de Documentacion Empleados livent - Minexus.xlsx
+++ b/Analisis de Documentacion Empleados livent - Minexus.xlsx
@@ -138,6 +138,7 @@
   </si>
   <si>
     <t xml:space="preserve">
+ -Declaración de Salud Ocupacional: Documento fuera de vigencia.
  -Registro de conducir: Documento fuera de vigencia.
  -Recibo de sueldo: Documento fuera de vigencia.</t>
   </si>
@@ -1891,7 +1892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="008000"/>
+        <fgColor rgb="FF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -5861,7 +5862,10 @@
         <v>24</v>
       </c>
       <c r="F41" t="s" s="85">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="42">

</xml_diff>